<commit_message>
update critical pass check list
</commit_message>
<xml_diff>
--- a/Android.xlsx
+++ b/Android.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Material Design" sheetId="1" r:id="rId1"/>
     <sheet name="Android app quality" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -298,7 +298,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -716,7 +716,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -726,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>